<commit_message>
Actualización agregando cosas 2023
</commit_message>
<xml_diff>
--- a/data/educacion_complementaria.xlsx
+++ b/data/educacion_complementaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanl\Desktop\Moni_HV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Moni_HV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FDF54-C255-4564-9B63-0A2E64A69C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D462C741-0EC3-4DAD-A64F-C3A7CEB88836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="1995" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>what</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Chamber College</t>
+  </si>
+  <si>
+    <t>tendencias del campo de la comunicación estratégica</t>
   </si>
 </sst>
 </file>
@@ -972,19 +975,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1006,97 +1009,97 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>2019</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>2018</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1104,41 +1107,41 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>2018</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>2017</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1146,15 +1149,29 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2017</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>2016</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>